<commit_message>
Service layer and basic http request handling implement
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Slawfirm_Defensive_Clients.xlsx
+++ b/src/main/resources/static/Slawfirm_Defensive_Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/safakarsli/Desktop/Paralegal Stuff/task_auto/slawfirm-server/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA93AAA-AC81-764E-B9FB-318D7031FA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B29DB10-E951-CA46-8B5B-4205AC1667C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{414D14DD-F4C2-0746-8DC6-E417DF045B3E}"/>
+    <workbookView xWindow="37860" yWindow="2720" windowWidth="28040" windowHeight="17440" xr2:uid="{414D14DD-F4C2-0746-8DC6-E417DF045B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,12 +425,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +746,13 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -780,28 +781,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
-        <v>6000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>6000</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>45148</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>